<commit_message>
save and load 缺epocho连续
</commit_message>
<xml_diff>
--- a/Mycnn/Mycnn/全连接层分类.xlsx
+++ b/Mycnn/Mycnn/全连接层分类.xlsx
@@ -16,29 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <r>
-      <t>网络结构:784-128-64-12 Batch_Size=</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">网络结构:784-128-64-12  </t>
     </r>
     <r>
       <rPr>
@@ -50,19 +31,15 @@
       </rPr>
       <t xml:space="preserve">ReLU </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color theme="9"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Mean=0 dev =0.2</t>
-    </r>
+  </si>
+  <si>
+    <t>Batch_Size</t>
   </si>
   <si>
     <t>lr</t>
+  </si>
+  <si>
+    <t>(mean,var)</t>
   </si>
   <si>
     <t>Epochs</t>
@@ -85,6 +62,18 @@
   <si>
     <t>Time</t>
   </si>
+  <si>
+    <t>(0, 0.2)</t>
+  </si>
+  <si>
+    <t>(0, 0.1)</t>
+  </si>
+  <si>
+    <t>早早收敛，但是相同epoch下总耗时更长</t>
+  </si>
+  <si>
+    <t>（0, 0.2）</t>
+  </si>
 </sst>
 </file>
 
@@ -96,7 +85,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +102,23 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -268,26 +267,12 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFFF9900"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FFFF9900"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="9"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,66 +281,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -487,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -505,6 +502,43 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -628,55 +662,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -688,16 +719,13 @@
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -706,10 +734,10 @@
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -718,10 +746,10 @@
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -730,10 +758,10 @@
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -742,10 +770,10 @@
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -754,28 +782,43 @@
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -842,13 +885,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1878965</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>1206500</xdr:rowOff>
@@ -868,7 +911,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8662670" y="2555240"/>
+          <a:off x="13780770" y="2555240"/>
           <a:ext cx="1583690" cy="1191260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -880,13 +923,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>262890</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1846580</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>1210310</xdr:rowOff>
@@ -906,8 +949,236 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6529705" y="2559050"/>
+          <a:off x="11637645" y="2559050"/>
           <a:ext cx="1583690" cy="1191260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>39370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1904365</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1233170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1" descr="cr"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13806170" y="5119370"/>
+          <a:ext cx="1583690" cy="1193800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1847215</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1252855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2" descr="ls"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11638280" y="5140960"/>
+          <a:ext cx="1583690" cy="1191895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>302895</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1268095</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1886585</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1195070</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7" descr="cr0.01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13788390" y="8888095"/>
+          <a:ext cx="1583690" cy="1196975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>245745</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1829435</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1244600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8" descr="ls0.01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11620500" y="8937625"/>
+          <a:ext cx="1583690" cy="1196975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>259715</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76835</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1843405</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9" descr="cr0.01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13745210" y="11506835"/>
+          <a:ext cx="1583690" cy="1196975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1827530</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1214120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10" descr="ls0.01"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11618595" y="11445875"/>
+          <a:ext cx="1583690" cy="1198245"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1169,119 +1440,285 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:I6"/>
+  <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
+    <col min="2" max="2" width="22.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="16.25" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20.6296296296296" customWidth="1"/>
-    <col min="7" max="8" width="30.6296296296296" customWidth="1"/>
-    <col min="9" max="9" width="21.75" customWidth="1"/>
+    <col min="7" max="7" width="30.6296296296296" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6296296296296" customWidth="1"/>
+    <col min="9" max="10" width="30.7777777777778" customWidth="1"/>
+    <col min="11" max="11" width="20.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="100" customHeight="1" spans="2:9">
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="100" customHeight="1" spans="2:11">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
-    <row r="2" ht="100" customHeight="1" spans="2:9">
-      <c r="B2" s="2" t="s">
+    <row r="2" ht="100" customHeight="1" spans="2:11">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" ht="100" customHeight="1" spans="2:9">
-      <c r="B3" s="2">
+    <row r="3" ht="100" customHeight="1" spans="2:11">
+      <c r="B3" s="6">
+        <v>100</v>
+      </c>
+      <c r="C3" s="4">
         <v>0.01</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
         <v>200</v>
       </c>
-      <c r="D3" s="3">
+      <c r="F3" s="4">
         <v>1168.53166329036</v>
       </c>
-      <c r="E3" s="3">
+      <c r="G3" s="4">
         <v>0.811480321729419</v>
       </c>
-      <c r="F3" s="4">
+      <c r="H3" s="5">
         <v>0.780555555555555</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4">
         <v>654</v>
       </c>
     </row>
-    <row r="4" ht="100" customHeight="1" spans="2:9">
-      <c r="B4" s="2">
+    <row r="4" ht="100" customHeight="1" spans="2:11">
+      <c r="B4" s="7"/>
+      <c r="C4" s="4">
         <v>0.001</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4">
         <v>800</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
-    <row r="5" ht="100" customHeight="1" spans="2:9">
-      <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+    <row r="5" ht="100" customHeight="1" spans="2:11">
+      <c r="B5" s="7"/>
+      <c r="C5" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4">
+        <v>300</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1199.49112938986</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.832979950965186</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.822916666666666</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
+        <v>1012</v>
+      </c>
     </row>
-    <row r="6" ht="100" customHeight="1" spans="2:9">
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="6" ht="100" customHeight="1" spans="2:11">
+      <c r="B6" s="8"/>
+      <c r="C6" s="4">
+        <v>0.001</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4">
+        <v>600</v>
+      </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" ht="100" customHeight="1" spans="2:11">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="100" customHeight="1" spans="2:12">
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4">
+        <v>120</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1021.59644103401</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.70944197294029</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.853472222222222</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>980</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" ht="100" customHeight="1" spans="2:11">
+      <c r="B9" s="7"/>
+      <c r="C9" s="4">
+        <v>0.001</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" ht="100" customHeight="1" spans="2:11">
+      <c r="B10" s="7"/>
+      <c r="C10" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4">
+        <v>120</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1047.67137576166</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.727549566501156</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.871527777777777</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="11" ht="100" customHeight="1" spans="2:11">
+      <c r="B11" s="8"/>
+      <c r="C11" s="4">
+        <v>0.001</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>